<commit_message>
Altered user card counts to fix playtesting issues
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="200" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="11535" yWindow="195" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Infrastructure" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Application" sheetId="3" r:id="rId3"/>
     <sheet name="User" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -174,7 +174,10 @@
     <t>Social Media</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>Users Provided</t>
+  </si>
+  <si>
+    <t>Card Quantity</t>
   </si>
 </sst>
 </file>
@@ -227,6 +230,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -558,12 +566,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -594,7 +602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -608,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -622,7 +630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -639,7 +647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -656,7 +664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -691,12 +699,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
@@ -704,7 +712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +753,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -762,7 +770,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -779,7 +787,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -796,7 +804,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -816,7 +824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -839,7 +847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -856,7 +864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -873,7 +881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -908,12 +916,12 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
@@ -921,7 +929,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -965,7 +973,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -988,7 +996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1014,7 +1022,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1037,7 +1045,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1060,7 +1068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1083,7 +1091,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1106,7 +1114,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1129,7 +1137,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1158,7 +1166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1184,7 +1192,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1207,7 +1215,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1230,7 +1238,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1253,7 +1261,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1276,7 +1284,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1299,7 +1307,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1331,23 +1339,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1365,7 @@
         <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>30</v>
@@ -1373,154 +1383,320 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
       <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2</v>
+      </c>
       <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2</v>
+      </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2</v>
+      </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>21</v>
       </c>
       <c r="F9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>21</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2</v>
+      </c>
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
       <c r="H11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
       <c r="F12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>21</v>
       </c>
       <c r="H14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" t="s">
         <v>21</v>
       </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
       <c r="H16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1</v>
+      </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
       </c>
       <c r="G17" t="s">
         <v>21</v>
       </c>
       <c r="H17" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f>SUM(C5:C25)</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added names to User Cards
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +178,66 @@
   </si>
   <si>
     <t>Card Quantity</t>
+  </si>
+  <si>
+    <t>Bankers</t>
+  </si>
+  <si>
+    <t>Office Workers</t>
+  </si>
+  <si>
+    <t>Home Cinema Owners</t>
+  </si>
+  <si>
+    <t>MOOC Students</t>
+  </si>
+  <si>
+    <t>University Lecturers</t>
+  </si>
+  <si>
+    <t>Tele Workers</t>
+  </si>
+  <si>
+    <t>Market Researchers</t>
+  </si>
+  <si>
+    <t>Online shoppers</t>
+  </si>
+  <si>
+    <t>Free to Play Gamers</t>
+  </si>
+  <si>
+    <t>Workplace Gamers</t>
+  </si>
+  <si>
+    <t>Premium News Readers</t>
+  </si>
+  <si>
+    <t>Social Media Shills</t>
+  </si>
+  <si>
+    <t>Tele Working Consultants</t>
+  </si>
+  <si>
+    <t>Video Game Bloggers</t>
+  </si>
+  <si>
+    <t>Mash up Artists</t>
+  </si>
+  <si>
+    <t>Game Review Excessive</t>
+  </si>
+  <si>
+    <t>Creative Professionals</t>
+  </si>
+  <si>
+    <t>Fun loving socialites</t>
+  </si>
+  <si>
+    <t>University Researchers</t>
+  </si>
+  <si>
+    <t>Documentary Watchers</t>
   </si>
 </sst>
 </file>
@@ -913,7 +973,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1342,7 +1402,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1384,6 +1444,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
       <c r="B5">
         <v>2</v>
       </c>
@@ -1398,6 +1461,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
       <c r="B6">
         <v>2</v>
       </c>
@@ -1412,6 +1478,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
       <c r="B7">
         <v>2</v>
       </c>
@@ -1426,6 +1495,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
       <c r="B8">
         <v>2</v>
       </c>
@@ -1440,6 +1512,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
       <c r="B9">
         <v>2</v>
       </c>
@@ -1454,6 +1529,9 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
       <c r="B10">
         <v>2</v>
       </c>
@@ -1468,6 +1546,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
       <c r="B11">
         <v>2</v>
       </c>
@@ -1482,6 +1563,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
       <c r="B12">
         <v>2</v>
       </c>
@@ -1496,6 +1580,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
       <c r="B13">
         <v>2</v>
       </c>
@@ -1510,6 +1597,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
       <c r="B14">
         <v>2</v>
       </c>
@@ -1524,6 +1614,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
       <c r="B16">
         <v>1</v>
       </c>
@@ -1540,7 +1633,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
       <c r="B17">
         <v>1</v>
       </c>
@@ -1557,7 +1653,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
       <c r="B18">
         <v>1</v>
       </c>
@@ -1574,7 +1673,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
       <c r="B19">
         <v>1</v>
       </c>
@@ -1591,7 +1693,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
       <c r="B20">
         <v>1</v>
       </c>
@@ -1608,7 +1713,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
       <c r="B21">
         <v>1</v>
       </c>
@@ -1625,7 +1733,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
       <c r="B22">
         <v>1</v>
       </c>
@@ -1642,7 +1753,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
       <c r="B23">
         <v>1</v>
       </c>
@@ -1659,7 +1773,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
       <c r="B24">
         <v>1</v>
       </c>
@@ -1676,7 +1793,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
       <c r="B25">
         <v>1</v>
       </c>
@@ -1693,7 +1813,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28">
         <f>SUM(C5:C25)</f>
         <v>30</v>

</xml_diff>